<commit_message>
Updated test data for German,Czech market Added test data for Belgium market
</commit_message>
<xml_diff>
--- a/Test Data/AttachedFunctionality_PFI_Node.xlsx
+++ b/Test Data/AttachedFunctionality_PFI_Node.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C19E26-5BE2-42E9-A026-80417AC4826B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D908026-0F08-4712-BC6A-CD733C938CAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Attached Functionality" sheetId="7" r:id="rId1"/>
-    <sheet name="Attached Functionality xBB" sheetId="8" r:id="rId2"/>
-    <sheet name="Czech" sheetId="9" r:id="rId3"/>
-    <sheet name="CzechxBB" sheetId="10" r:id="rId4"/>
+    <sheet name="Germany" sheetId="7" r:id="rId1"/>
+    <sheet name="GermanyxBB" sheetId="8" r:id="rId2"/>
+    <sheet name="Belgium" sheetId="11" r:id="rId3"/>
+    <sheet name="BelgiumxBB" sheetId="12" r:id="rId4"/>
+    <sheet name="Czech" sheetId="9" r:id="rId5"/>
+    <sheet name="CzechxBB" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="22">
   <si>
     <t>Wg</t>
   </si>
@@ -96,6 +98,12 @@
   </si>
   <si>
     <t>NGC-3477/T1736</t>
+  </si>
+  <si>
+    <t>Belgium Market</t>
+  </si>
+  <si>
+    <t>NGC-3478/T2266</t>
   </si>
 </sst>
 </file>
@@ -520,7 +528,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -755,11 +763,250 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B44514F-4CC4-48ED-BF22-A9302AF78CC7}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="42.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30984FFC-D37F-4291-9644-30326B87624C}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="42.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D721F631-0412-46FD-91E9-9CC64B2F261B}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -870,11 +1117,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{736FEEC1-2829-49BB-B9C3-5C3559582F7C}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added test data for Switzerland market
</commit_message>
<xml_diff>
--- a/Test Data/AttachedFunctionality_PFI_Node.xlsx
+++ b/Test Data/AttachedFunctionality_PFI_Node.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D908026-0F08-4712-BC6A-CD733C938CAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5DF632-B5B9-4D9A-AE80-141C9282979A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
   <sheets>
     <sheet name="Germany" sheetId="7" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="BelgiumxBB" sheetId="12" r:id="rId4"/>
     <sheet name="Czech" sheetId="9" r:id="rId5"/>
     <sheet name="CzechxBB" sheetId="10" r:id="rId6"/>
+    <sheet name="Swiss" sheetId="14" r:id="rId7"/>
+    <sheet name="SwissBB" sheetId="13" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="25">
   <si>
     <t>Wg</t>
   </si>
@@ -104,6 +106,15 @@
   </si>
   <si>
     <t>NGC-3478/T2266</t>
+  </si>
+  <si>
+    <t>Switzerland Market</t>
+  </si>
+  <si>
+    <t>NGC-3476/T2351</t>
+  </si>
+  <si>
+    <t>Fire Brigade Panel - LocalIO</t>
   </si>
 </sst>
 </file>
@@ -645,7 +656,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1005,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D721F631-0412-46FD-91E9-9CC64B2F261B}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1122,7 +1133,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1236,4 +1247,221 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91578DB-01A1-487C-A9DB-633CB8D15A1E}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="41.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="26.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A6B98A-6404-4D9E-B25F-C3C2229080D6}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="41.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated TestData for Portugal Market
</commit_message>
<xml_diff>
--- a/Test Data/AttachedFunctionality_PFI_Node.xlsx
+++ b/Test Data/AttachedFunctionality_PFI_Node.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5DF632-B5B9-4D9A-AE80-141C9282979A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64E2C30-7BC0-4B56-A08C-7A7441EE7E1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="9" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
   <sheets>
     <sheet name="Germany" sheetId="7" r:id="rId1"/>
@@ -21,6 +21,8 @@
     <sheet name="CzechxBB" sheetId="10" r:id="rId6"/>
     <sheet name="Swiss" sheetId="14" r:id="rId7"/>
     <sheet name="SwissBB" sheetId="13" r:id="rId8"/>
+    <sheet name="Portugal" sheetId="16" r:id="rId9"/>
+    <sheet name="PortugalBB" sheetId="17" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="27">
   <si>
     <t>Wg</t>
   </si>
@@ -115,6 +117,12 @@
   </si>
   <si>
     <t>Fire Brigade Panel - LocalIO</t>
+  </si>
+  <si>
+    <t>Portugal Market</t>
+  </si>
+  <si>
+    <t>NGC-3479/T2407</t>
   </si>
 </sst>
 </file>
@@ -651,6 +659,128 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{735F00D8-059C-4708-A23F-15C6882E7CED}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="41" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E93295D-FD1C-46C7-814A-7EEF4111103A}">
   <dimension ref="A1:D15"/>
@@ -778,7 +908,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection sqref="A1:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -895,7 +1025,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection sqref="A1:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1359,7 +1489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A6B98A-6404-4D9E-B25F-C3C2229080D6}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -1464,4 +1594,121 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{892A6D6F-41E4-430E-BE09-BAD7BBFD4F21}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40.88671875" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test Data Added for Slovakia market
</commit_message>
<xml_diff>
--- a/Test Data/AttachedFunctionality_PFI_Node.xlsx
+++ b/Test Data/AttachedFunctionality_PFI_Node.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64E2C30-7BC0-4B56-A08C-7A7441EE7E1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F0AD51-7C20-499D-B823-4FB379109702}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="9" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="10" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
   <sheets>
     <sheet name="Germany" sheetId="7" r:id="rId1"/>
@@ -23,6 +23,8 @@
     <sheet name="SwissBB" sheetId="13" r:id="rId8"/>
     <sheet name="Portugal" sheetId="16" r:id="rId9"/>
     <sheet name="PortugalBB" sheetId="17" r:id="rId10"/>
+    <sheet name="Slovakia" sheetId="18" r:id="rId11"/>
+    <sheet name="SlovakiaxBB" sheetId="19" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="29">
   <si>
     <t>Wg</t>
   </si>
@@ -123,6 +125,12 @@
   </si>
   <si>
     <t>NGC-3479/T2407</t>
+  </si>
+  <si>
+    <t>Slovakia Market</t>
+  </si>
+  <si>
+    <t>NGC-2930/T3223</t>
   </si>
 </sst>
 </file>
@@ -547,7 +555,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -663,7 +671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{735F00D8-059C-4708-A23F-15C6882E7CED}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -718,6 +726,245 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7A264D2-E89D-48C6-A7A3-1A90B154F27F}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="42.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B8F789-7AFC-404E-9230-23453833DBB7}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="42.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C5" s="6"/>
       <c r="D5" s="2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Test data added for Italy
</commit_message>
<xml_diff>
--- a/Test Data/AttachedFunctionality_PFI_Node.xlsx
+++ b/Test Data/AttachedFunctionality_PFI_Node.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F0AD51-7C20-499D-B823-4FB379109702}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DE4022-322E-4EC3-B641-B4B9F65A18A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="10" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="12" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
   <sheets>
     <sheet name="Germany" sheetId="7" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="PortugalBB" sheetId="17" r:id="rId10"/>
     <sheet name="Slovakia" sheetId="18" r:id="rId11"/>
     <sheet name="SlovakiaxBB" sheetId="19" r:id="rId12"/>
+    <sheet name="Italy" sheetId="20" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="31">
   <si>
     <t>Wg</t>
   </si>
@@ -131,6 +132,12 @@
   </si>
   <si>
     <t>NGC-2930/T3223</t>
+  </si>
+  <si>
+    <t>NGC-3145/T2157</t>
+  </si>
+  <si>
+    <t>Italy Market</t>
   </si>
 </sst>
 </file>
@@ -793,7 +800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7A264D2-E89D-48C6-A7A3-1A90B154F27F}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -911,7 +918,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1015,6 +1022,108 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB8AC07-1ADC-41C0-94BD-25856535D12F}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40.88671875" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1848,7 +1957,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B5"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added Test data for Spain Zettler Market
</commit_message>
<xml_diff>
--- a/Test Data/AttachedFunctionality_PFI_Node.xlsx
+++ b/Test Data/AttachedFunctionality_PFI_Node.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DE4022-322E-4EC3-B641-B4B9F65A18A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{253759DA-7E50-4B62-A278-D360892C152B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="12" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="13" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
   <sheets>
     <sheet name="Germany" sheetId="7" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="Slovakia" sheetId="18" r:id="rId11"/>
     <sheet name="SlovakiaxBB" sheetId="19" r:id="rId12"/>
     <sheet name="Italy" sheetId="20" r:id="rId13"/>
+    <sheet name="Spain" sheetId="21" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="33">
   <si>
     <t>Wg</t>
   </si>
@@ -138,6 +139,12 @@
   </si>
   <si>
     <t>Italy Market</t>
+  </si>
+  <si>
+    <t>NGC-3103/T2041</t>
+  </si>
+  <si>
+    <t>Spain Market</t>
   </si>
 </sst>
 </file>
@@ -1039,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB8AC07-1ADC-41C0-94BD-25856535D12F}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1094,6 +1101,107 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A92F6D8-F197-4E68-810F-5255086BBCCE}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C5" s="6"/>
       <c r="D5" s="2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Added Test data for Turkey Template for Zettler
</commit_message>
<xml_diff>
--- a/Test Data/AttachedFunctionality_PFI_Node.xlsx
+++ b/Test Data/AttachedFunctionality_PFI_Node.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{253759DA-7E50-4B62-A278-D360892C152B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A036C61-D0D1-4182-870C-D302FA9E126B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="13" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="14" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
   <sheets>
     <sheet name="Germany" sheetId="7" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="SlovakiaxBB" sheetId="19" r:id="rId12"/>
     <sheet name="Italy" sheetId="20" r:id="rId13"/>
     <sheet name="Spain" sheetId="21" r:id="rId14"/>
+    <sheet name="Turkey" sheetId="22" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="35">
   <si>
     <t>Wg</t>
   </si>
@@ -145,6 +146,12 @@
   </si>
   <si>
     <t>Spain Market</t>
+  </si>
+  <si>
+    <t>Turkey Market</t>
+  </si>
+  <si>
+    <t>NGC-3191/T3299</t>
   </si>
 </sst>
 </file>
@@ -1148,8 +1155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A92F6D8-F197-4E68-810F-5255086BBCCE}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1202,6 +1209,107 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{995EA6ED-67A3-4D67-80CF-A54DEEC7B4AE}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C5" s="6"/>
       <c r="D5" s="2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Added Test Data for Croatia Market
</commit_message>
<xml_diff>
--- a/Test Data/AttachedFunctionality_PFI_Node.xlsx
+++ b/Test Data/AttachedFunctionality_PFI_Node.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A036C61-D0D1-4182-870C-D302FA9E126B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316B438B-7F85-4EC8-BF3E-9B8C988E393F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="14" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="15" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
   <sheets>
     <sheet name="Germany" sheetId="7" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <sheet name="Italy" sheetId="20" r:id="rId13"/>
     <sheet name="Spain" sheetId="21" r:id="rId14"/>
     <sheet name="Turkey" sheetId="22" r:id="rId15"/>
+    <sheet name="Croatia" sheetId="23" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="37">
   <si>
     <t>Wg</t>
   </si>
@@ -152,6 +153,12 @@
   </si>
   <si>
     <t>NGC-3191/T3299</t>
+  </si>
+  <si>
+    <t>Croatia Market</t>
+  </si>
+  <si>
+    <t>NGC-3139/T2421</t>
   </si>
 </sst>
 </file>
@@ -1256,8 +1263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{995EA6ED-67A3-4D67-80CF-A54DEEC7B4AE}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1310,6 +1317,107 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E669DD6E-BBFE-425A-BE31-CE34F77D6C82}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C5" s="6"/>
       <c r="D5" s="2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Test data for Greece Market
</commit_message>
<xml_diff>
--- a/Test Data/AttachedFunctionality_PFI_Node.xlsx
+++ b/Test Data/AttachedFunctionality_PFI_Node.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316B438B-7F85-4EC8-BF3E-9B8C988E393F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164D54AD-3563-4CC5-8E5D-BE8EB5AC68BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="15" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="16" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
   <sheets>
     <sheet name="Germany" sheetId="7" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <sheet name="Spain" sheetId="21" r:id="rId14"/>
     <sheet name="Turkey" sheetId="22" r:id="rId15"/>
     <sheet name="Croatia" sheetId="23" r:id="rId16"/>
+    <sheet name="Greece" sheetId="24" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="39">
   <si>
     <t>Wg</t>
   </si>
@@ -159,6 +160,12 @@
   </si>
   <si>
     <t>NGC-3139/T2421</t>
+  </si>
+  <si>
+    <t>Greece Market</t>
+  </si>
+  <si>
+    <t>NGC-4119/T3168</t>
   </si>
 </sst>
 </file>
@@ -1364,6 +1371,107 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E669DD6E-BBFE-425A-BE31-CE34F77D6C82}">
   <dimension ref="A1:D11"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C3C2C3-5921-4988-8716-D8A09E2E85A7}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
@@ -1388,7 +1496,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>3</v>
@@ -1410,7 +1518,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="2" t="s">

</xml_diff>

<commit_message>
Test data for Austria market added
</commit_message>
<xml_diff>
--- a/Test Data/AttachedFunctionality_PFI_Node.xlsx
+++ b/Test Data/AttachedFunctionality_PFI_Node.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164D54AD-3563-4CC5-8E5D-BE8EB5AC68BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04897392-671B-4194-B970-3273AB929FAA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="16" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="10" activeTab="19" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
   <sheets>
     <sheet name="Germany" sheetId="7" r:id="rId1"/>
@@ -30,6 +30,9 @@
     <sheet name="Turkey" sheetId="22" r:id="rId15"/>
     <sheet name="Croatia" sheetId="23" r:id="rId16"/>
     <sheet name="Greece" sheetId="24" r:id="rId17"/>
+    <sheet name="Netherlands" sheetId="25" r:id="rId18"/>
+    <sheet name="Denmark" sheetId="27" r:id="rId19"/>
+    <sheet name="Austria" sheetId="26" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="47">
   <si>
     <t>Wg</t>
   </si>
@@ -166,6 +169,30 @@
   </si>
   <si>
     <t>NGC-4119/T3168</t>
+  </si>
+  <si>
+    <t>Netherlands Market</t>
+  </si>
+  <si>
+    <t>NGC-3144/T2183</t>
+  </si>
+  <si>
+    <t>Austria Market</t>
+  </si>
+  <si>
+    <t>Multichannel Transmission Unit</t>
+  </si>
+  <si>
+    <t>Transmission Unit and Keysafe</t>
+  </si>
+  <si>
+    <t>NGC-3817/T2279</t>
+  </si>
+  <si>
+    <t>Denmark Market</t>
+  </si>
+  <si>
+    <t>NGC-2913/T2183</t>
   </si>
 </sst>
 </file>
@@ -1472,7 +1499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C3C2C3-5921-4988-8716-D8A09E2E85A7}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1526,6 +1553,210 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{175060A6-476D-46A9-BCA2-2DA0D645364E}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40.88671875" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB3B3109-CF5E-4FCE-BDAE-7CF9ABE64BD0}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40.88671875" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C5" s="6"/>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -1691,6 +1922,128 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C84095E2-890B-48B0-8088-2C15865EAD8C}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="43.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B44514F-4CC4-48ED-BF22-A9302AF78CC7}">
   <dimension ref="A1:D14"/>

</xml_diff>

<commit_message>
Test data for Netherlands And Denmark market added
</commit_message>
<xml_diff>
--- a/Test Data/AttachedFunctionality_PFI_Node.xlsx
+++ b/Test Data/AttachedFunctionality_PFI_Node.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04897392-671B-4194-B970-3273AB929FAA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B27AFA5-84BB-4FD6-AB2A-976F60132580}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="10" activeTab="19" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="48">
   <si>
     <t>Wg</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>NGC-2913/T2183</t>
+  </si>
+  <si>
+    <t>Multichannel Transmission Unit and Keysafe</t>
   </si>
 </sst>
 </file>
@@ -1927,7 +1930,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2021,7 +2024,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added Test Data For Hungary/Russia/Finland Market
</commit_message>
<xml_diff>
--- a/Test Data/AttachedFunctionality_PFI_Node.xlsx
+++ b/Test Data/AttachedFunctionality_PFI_Node.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B27AFA5-84BB-4FD6-AB2A-976F60132580}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F81EF4-FDB1-4B7F-95BB-3591E9306519}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="10" activeTab="19" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="13" activeTab="15" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
   <sheets>
     <sheet name="Germany" sheetId="7" r:id="rId1"/>
@@ -33,6 +33,9 @@
     <sheet name="Netherlands" sheetId="25" r:id="rId18"/>
     <sheet name="Denmark" sheetId="27" r:id="rId19"/>
     <sheet name="Austria" sheetId="26" r:id="rId20"/>
+    <sheet name="Russia" sheetId="29" r:id="rId21"/>
+    <sheet name="Finland" sheetId="30" r:id="rId22"/>
+    <sheet name="Hungary" sheetId="31" r:id="rId23"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="54">
   <si>
     <t>Wg</t>
   </si>
@@ -196,6 +199,24 @@
   </si>
   <si>
     <t>Multichannel Transmission Unit and Keysafe</t>
+  </si>
+  <si>
+    <t>NGC-2929/T2901</t>
+  </si>
+  <si>
+    <t>Russia Market</t>
+  </si>
+  <si>
+    <t>NGC-3130/T2944</t>
+  </si>
+  <si>
+    <t>Finland Market</t>
+  </si>
+  <si>
+    <t>NGC-3104/T2993</t>
+  </si>
+  <si>
+    <t>Hungary Market</t>
   </si>
 </sst>
 </file>
@@ -1401,8 +1422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E669DD6E-BBFE-425A-BE31-CE34F77D6C82}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1929,7 +1950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C84095E2-890B-48B0-8088-2C15865EAD8C}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -2034,6 +2055,309 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01B99D09-21B4-46C8-BF94-A63DC02FAD82}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE39BC62-4114-4FED-B6A2-2EF3389B68DD}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9AF15AE-7701-4DA0-A558-740FD8D9B32E}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Test data For Norway and Poland Market
</commit_message>
<xml_diff>
--- a/Test Data/AttachedFunctionality_PFI_Node.xlsx
+++ b/Test Data/AttachedFunctionality_PFI_Node.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F81EF4-FDB1-4B7F-95BB-3591E9306519}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA898BE4-9143-46C2-BAAC-4BDEE4A6C709}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="13" activeTab="15" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="13" activeTab="23" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
   <sheets>
     <sheet name="Germany" sheetId="7" r:id="rId1"/>
@@ -36,6 +36,8 @@
     <sheet name="Russia" sheetId="29" r:id="rId21"/>
     <sheet name="Finland" sheetId="30" r:id="rId22"/>
     <sheet name="Hungary" sheetId="31" r:id="rId23"/>
+    <sheet name="Norway" sheetId="33" r:id="rId24"/>
+    <sheet name="Poland" sheetId="34" r:id="rId25"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="58">
   <si>
     <t>Wg</t>
   </si>
@@ -217,6 +219,18 @@
   </si>
   <si>
     <t>Hungary Market</t>
+  </si>
+  <si>
+    <t>NGC-2931/T3062</t>
+  </si>
+  <si>
+    <t>Norway Market</t>
+  </si>
+  <si>
+    <t>NGC-2920/T3105</t>
+  </si>
+  <si>
+    <t>Poland Market</t>
   </si>
 </sst>
 </file>
@@ -1422,7 +1436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E669DD6E-BBFE-425A-BE31-CE34F77D6C82}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -2371,6 +2385,208 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6B3BD8A-CD3A-4AFF-8BB0-7C3FB0729C34}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C25BABA6-9241-439D-A852-DF46B9EC5A57}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B44514F-4CC4-48ED-BF22-A9302AF78CC7}">
   <dimension ref="A1:D14"/>

</xml_diff>

<commit_message>
Added Test Data for UK Market
</commit_message>
<xml_diff>
--- a/Test Data/AttachedFunctionality_PFI_Node.xlsx
+++ b/Test Data/AttachedFunctionality_PFI_Node.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA898BE4-9143-46C2-BAAC-4BDEE4A6C709}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17F9EF7-F72F-4D25-9FA4-144C3A7318C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="13" activeTab="23" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="15" activeTab="25" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
   <sheets>
     <sheet name="Germany" sheetId="7" r:id="rId1"/>
@@ -38,6 +38,7 @@
     <sheet name="Hungary" sheetId="31" r:id="rId23"/>
     <sheet name="Norway" sheetId="33" r:id="rId24"/>
     <sheet name="Poland" sheetId="34" r:id="rId25"/>
+    <sheet name="UK" sheetId="35" r:id="rId26"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="60">
   <si>
     <t>Wg</t>
   </si>
@@ -231,6 +232,12 @@
   </si>
   <si>
     <t>Poland Market</t>
+  </si>
+  <si>
+    <t>NGC-2741/T3344</t>
+  </si>
+  <si>
+    <t>UK Market</t>
   </si>
 </sst>
 </file>
@@ -2389,7 +2396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6B3BD8A-CD3A-4AFF-8BB0-7C3FB0729C34}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -2537,6 +2544,107 @@
       </c>
       <c r="B4" t="s">
         <v>56</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD88C6AE-BDEB-4358-9F04-8CAD26DBB10A}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="2" t="s">

</xml_diff>